<commit_message>
ya todo rerminado :)
</commit_message>
<xml_diff>
--- a/Empleados.xlsx
+++ b/Empleados.xlsx
@@ -464,7 +464,7 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
     <col width="16.453125" customWidth="1" min="2" max="2"/>
     <col width="24.54296875" customWidth="1" min="3" max="3"/>
@@ -509,10 +509,8 @@
           <t>DESCUENTO</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>SUELDO_QUIN</t>
-        </is>
+      <c r="H1" s="1" t="n">
+        <v>21000</v>
       </c>
     </row>
     <row r="2">
@@ -542,6 +540,12 @@
       <c r="F2" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="G2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>18900</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -570,6 +574,9 @@
       <c r="F3" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="H3" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -598,6 +605,9 @@
       <c r="F4" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="H4" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -626,6 +636,9 @@
       <c r="F5" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H5" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -654,6 +667,9 @@
       <c r="F6" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="H6" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -682,6 +698,12 @@
       <c r="F7" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="G7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>18900</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -710,6 +732,9 @@
       <c r="F8" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H8" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -738,6 +763,9 @@
       <c r="F9" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H9" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -766,6 +794,9 @@
       <c r="F10" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H10" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -794,6 +825,9 @@
       <c r="F11" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="H11" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -822,6 +856,9 @@
       <c r="F12" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="H12" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -850,6 +887,9 @@
       <c r="F13" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="H13" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -878,6 +918,9 @@
       <c r="F14" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="H14" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -906,6 +949,9 @@
       <c r="F15" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="H15" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -934,6 +980,9 @@
       <c r="F16" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H16" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -962,6 +1011,9 @@
       <c r="F17" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H17" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -990,6 +1042,9 @@
       <c r="F18" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H18" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1018,6 +1073,9 @@
       <c r="F19" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="H19" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1046,6 +1104,9 @@
       <c r="F20" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="H20" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1074,6 +1135,9 @@
       <c r="F21" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H21" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1102,6 +1166,9 @@
       <c r="F22" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="H22" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1130,6 +1197,9 @@
       <c r="F23" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H23" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1158,6 +1228,9 @@
       <c r="F24" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H24" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1186,6 +1259,9 @@
       <c r="F25" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="H25" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1205,14 +1281,17 @@
       </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>I</t>
         </is>
       </c>
       <c r="E26" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F26" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>21000</v>
       </c>
     </row>
     <row r="27">
@@ -1242,6 +1321,12 @@
       <c r="F27" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="G27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>18900</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1270,6 +1355,9 @@
       <c r="F28" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H28" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1298,6 +1386,9 @@
       <c r="F29" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="H29" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1326,6 +1417,12 @@
       <c r="F30" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="G30" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H30" t="n">
+        <v>18900</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1354,6 +1451,12 @@
       <c r="F31" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="G31" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H31" t="n">
+        <v>18900</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1382,6 +1485,9 @@
       <c r="F32" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="H32" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1410,6 +1516,9 @@
       <c r="F33" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="H33" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1438,6 +1547,9 @@
       <c r="F34" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="H34" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1466,6 +1578,9 @@
       <c r="F35" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="H35" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1494,6 +1609,9 @@
       <c r="F36" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="H36" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1522,6 +1640,12 @@
       <c r="F37" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="G37" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H37" t="n">
+        <v>18900</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1550,6 +1674,12 @@
       <c r="F38" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="G38" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H38" t="n">
+        <v>18900</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1578,6 +1708,12 @@
       <c r="F39" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="G39" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H39" t="n">
+        <v>18900</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1606,6 +1742,9 @@
       <c r="F40" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="H40" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1625,6 +1764,9 @@
       </c>
       <c r="D41" s="1" t="n"/>
       <c r="F41" s="2" t="n"/>
+      <c r="H41" t="n">
+        <v>21000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
viendo algo nuevo que me dijo armando
</commit_message>
<xml_diff>
--- a/Empleados.xlsx
+++ b/Empleados.xlsx
@@ -458,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
@@ -1768,6 +1768,34 @@
         <v>21000</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>385580</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Pepe</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Pelele</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>